<commit_message>
Started doing some measurements
</commit_message>
<xml_diff>
--- a/doc/Sprint_1/1222123/Measurements_Building2.xlsx
+++ b/doc/Sprint_1/1222123/Measurements_Building2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\Desktop\rcomp-dg-g1\doc\Sprint_1\1222123\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A86E2B6-90F5-4451-B7AC-EF584C687D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33374A54-7688-4B83-849C-438CC53D7582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{933D9862-C879-4DBF-8626-28FC115C8F48}"/>
   </bookViews>
@@ -293,7 +293,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,6 +311,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -383,7 +391,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
@@ -395,6 +403,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1590,6 +1599,7 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
+      <c r="H12" s="5"/>
     </row>
     <row r="13" spans="2:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">

</xml_diff>

<commit_message>
cabling and readme changes
</commit_message>
<xml_diff>
--- a/doc/Sprint_1/1222123/Measurements_Building2.xlsx
+++ b/doc/Sprint_1/1222123/Measurements_Building2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\Desktop\rcomp-dg-g1\doc\Sprint_1\1222123\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9C32B2-965A-4026-BCC4-9F7AE86E2C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81E0157-C183-44E7-AE11-D55017B53AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{933D9862-C879-4DBF-8626-28FC115C8F48}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{933D9862-C879-4DBF-8626-28FC115C8F48}"/>
   </bookViews>
   <sheets>
     <sheet name="Cable Measurements" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="89">
   <si>
     <t>Rooms</t>
   </si>
@@ -783,8 +783,8 @@
   <sheetPr codeName="Folha1"/>
   <dimension ref="B1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,7 +901,9 @@
       <c r="D11" s="1">
         <v>6</v>
       </c>
-      <c r="G11" s="1"/>
+      <c r="G11" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="H11" s="1" t="s">
         <v>13</v>
       </c>
@@ -918,7 +920,9 @@
       <c r="D12" s="1">
         <v>4</v>
       </c>
-      <c r="G12" s="1"/>
+      <c r="G12" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="H12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1212,6 +1216,11 @@
     <row r="37" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="O4:P4"/>
     <mergeCell ref="I10:J10"/>
     <mergeCell ref="G18:K18"/>
     <mergeCell ref="G9:J9"/>
@@ -1227,11 +1236,6 @@
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="I14:J14"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="O4:P4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1545,53 +1549,6 @@
     <row r="31" spans="9:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I3:L3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="I29:J29"/>
     <mergeCell ref="I30:J30"/>
     <mergeCell ref="K25:L25"/>
     <mergeCell ref="K10:L10"/>
@@ -1608,12 +1565,59 @@
     <mergeCell ref="K18:L18"/>
     <mergeCell ref="K17:L17"/>
     <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="I29:J29"/>
     <mergeCell ref="K24:L24"/>
     <mergeCell ref="K23:L23"/>
     <mergeCell ref="K22:L22"/>
     <mergeCell ref="K21:L21"/>
     <mergeCell ref="K20:L20"/>
     <mergeCell ref="K19:L19"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3295,160 +3299,166 @@
     <row r="182" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="352">
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="B98:C98"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="D56:F56"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="B118:C118"/>
-    <mergeCell ref="B119:C119"/>
-    <mergeCell ref="B120:C120"/>
-    <mergeCell ref="B121:C121"/>
-    <mergeCell ref="B122:C122"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="D126:F126"/>
-    <mergeCell ref="D127:F127"/>
-    <mergeCell ref="D128:F128"/>
-    <mergeCell ref="D129:F129"/>
-    <mergeCell ref="D130:F130"/>
-    <mergeCell ref="D131:F131"/>
-    <mergeCell ref="B124:C124"/>
-    <mergeCell ref="B125:C125"/>
-    <mergeCell ref="B126:C126"/>
-    <mergeCell ref="B127:C127"/>
-    <mergeCell ref="B128:C128"/>
-    <mergeCell ref="B129:C129"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="B131:C131"/>
-    <mergeCell ref="B141:C141"/>
-    <mergeCell ref="D141:F141"/>
-    <mergeCell ref="B132:C132"/>
-    <mergeCell ref="D132:F132"/>
-    <mergeCell ref="D133:F133"/>
-    <mergeCell ref="D134:F134"/>
-    <mergeCell ref="D135:F135"/>
-    <mergeCell ref="D136:F136"/>
-    <mergeCell ref="D137:F137"/>
-    <mergeCell ref="D138:F138"/>
-    <mergeCell ref="D139:F139"/>
-    <mergeCell ref="D140:F140"/>
-    <mergeCell ref="B133:C133"/>
-    <mergeCell ref="B134:C134"/>
-    <mergeCell ref="B135:C135"/>
-    <mergeCell ref="B136:C136"/>
-    <mergeCell ref="B137:C137"/>
-    <mergeCell ref="B138:C138"/>
-    <mergeCell ref="B139:C139"/>
-    <mergeCell ref="B140:C140"/>
-    <mergeCell ref="D142:F142"/>
-    <mergeCell ref="D143:F143"/>
-    <mergeCell ref="D144:F144"/>
-    <mergeCell ref="D145:F145"/>
-    <mergeCell ref="D146:F146"/>
-    <mergeCell ref="D147:F147"/>
-    <mergeCell ref="D148:F148"/>
-    <mergeCell ref="D149:F149"/>
-    <mergeCell ref="B142:C142"/>
-    <mergeCell ref="B143:C143"/>
-    <mergeCell ref="B144:C144"/>
-    <mergeCell ref="B145:C145"/>
-    <mergeCell ref="B146:C146"/>
-    <mergeCell ref="B147:C147"/>
-    <mergeCell ref="B148:C148"/>
-    <mergeCell ref="B149:C149"/>
-    <mergeCell ref="B157:C157"/>
-    <mergeCell ref="D157:F157"/>
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="D150:F150"/>
-    <mergeCell ref="B151:C151"/>
-    <mergeCell ref="B152:C152"/>
-    <mergeCell ref="B153:C153"/>
-    <mergeCell ref="B154:C154"/>
-    <mergeCell ref="B155:C155"/>
-    <mergeCell ref="B156:C156"/>
-    <mergeCell ref="D151:F151"/>
-    <mergeCell ref="D152:F152"/>
-    <mergeCell ref="D153:F153"/>
-    <mergeCell ref="D154:F154"/>
-    <mergeCell ref="D155:F155"/>
-    <mergeCell ref="D156:F156"/>
-    <mergeCell ref="B162:C162"/>
-    <mergeCell ref="D162:F162"/>
-    <mergeCell ref="B158:C158"/>
-    <mergeCell ref="B159:C159"/>
-    <mergeCell ref="B160:C160"/>
-    <mergeCell ref="B161:C161"/>
-    <mergeCell ref="D158:F158"/>
-    <mergeCell ref="D159:F159"/>
-    <mergeCell ref="D160:F160"/>
-    <mergeCell ref="D161:F161"/>
-    <mergeCell ref="B163:C163"/>
-    <mergeCell ref="B164:C164"/>
-    <mergeCell ref="B165:C165"/>
-    <mergeCell ref="B166:C166"/>
-    <mergeCell ref="B167:C167"/>
-    <mergeCell ref="B168:C168"/>
-    <mergeCell ref="B169:C169"/>
-    <mergeCell ref="B170:C170"/>
-    <mergeCell ref="D163:F163"/>
-    <mergeCell ref="D164:F164"/>
-    <mergeCell ref="D165:F165"/>
-    <mergeCell ref="D166:F166"/>
-    <mergeCell ref="D167:F167"/>
-    <mergeCell ref="D168:F168"/>
-    <mergeCell ref="D169:F169"/>
-    <mergeCell ref="D170:F170"/>
-    <mergeCell ref="B179:C179"/>
-    <mergeCell ref="B180:C180"/>
-    <mergeCell ref="B181:C181"/>
-    <mergeCell ref="D172:F172"/>
-    <mergeCell ref="D173:F173"/>
-    <mergeCell ref="D174:F174"/>
-    <mergeCell ref="D175:F175"/>
-    <mergeCell ref="D176:F176"/>
-    <mergeCell ref="D177:F177"/>
-    <mergeCell ref="D178:F178"/>
-    <mergeCell ref="D179:F179"/>
-    <mergeCell ref="D180:F180"/>
-    <mergeCell ref="D181:F181"/>
-    <mergeCell ref="B171:C171"/>
-    <mergeCell ref="D171:F171"/>
-    <mergeCell ref="B172:C172"/>
-    <mergeCell ref="B173:C173"/>
-    <mergeCell ref="B174:C174"/>
-    <mergeCell ref="B175:C175"/>
-    <mergeCell ref="B176:C176"/>
-    <mergeCell ref="B177:C177"/>
-    <mergeCell ref="B178:C178"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="D50:F50"/>
-    <mergeCell ref="D51:F51"/>
-    <mergeCell ref="D52:F52"/>
+    <mergeCell ref="D122:F122"/>
+    <mergeCell ref="D123:F123"/>
+    <mergeCell ref="D124:F124"/>
+    <mergeCell ref="D125:F125"/>
+    <mergeCell ref="D113:F113"/>
+    <mergeCell ref="D114:F114"/>
+    <mergeCell ref="D115:F115"/>
+    <mergeCell ref="D117:F117"/>
+    <mergeCell ref="D118:F118"/>
+    <mergeCell ref="D119:F119"/>
+    <mergeCell ref="D121:F121"/>
+    <mergeCell ref="D110:F110"/>
+    <mergeCell ref="D112:F112"/>
+    <mergeCell ref="D103:F103"/>
+    <mergeCell ref="D104:F104"/>
+    <mergeCell ref="D105:F105"/>
+    <mergeCell ref="D107:F107"/>
+    <mergeCell ref="D108:F108"/>
+    <mergeCell ref="D109:F109"/>
+    <mergeCell ref="D120:F120"/>
+    <mergeCell ref="D95:F95"/>
+    <mergeCell ref="D97:F97"/>
+    <mergeCell ref="D83:F83"/>
+    <mergeCell ref="D84:F84"/>
+    <mergeCell ref="D85:F85"/>
+    <mergeCell ref="D87:F87"/>
+    <mergeCell ref="D88:F88"/>
+    <mergeCell ref="D89:F89"/>
+    <mergeCell ref="D96:F96"/>
+    <mergeCell ref="D86:F86"/>
+    <mergeCell ref="D91:F91"/>
+    <mergeCell ref="D81:F81"/>
+    <mergeCell ref="D70:F70"/>
+    <mergeCell ref="D72:F72"/>
+    <mergeCell ref="D73:F73"/>
+    <mergeCell ref="D74:F74"/>
+    <mergeCell ref="D90:F90"/>
+    <mergeCell ref="D92:F92"/>
+    <mergeCell ref="D93:F93"/>
+    <mergeCell ref="D94:F94"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="D60:F60"/>
+    <mergeCell ref="D57:F57"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="D62:F62"/>
+    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="D54:F54"/>
+    <mergeCell ref="D55:F55"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="D101:F101"/>
+    <mergeCell ref="D106:F106"/>
+    <mergeCell ref="D111:F111"/>
+    <mergeCell ref="D116:F116"/>
+    <mergeCell ref="D98:F98"/>
+    <mergeCell ref="D99:F99"/>
+    <mergeCell ref="D100:F100"/>
+    <mergeCell ref="D102:F102"/>
+    <mergeCell ref="D75:F75"/>
+    <mergeCell ref="D77:F77"/>
+    <mergeCell ref="D78:F78"/>
+    <mergeCell ref="D79:F79"/>
+    <mergeCell ref="D80:F80"/>
+    <mergeCell ref="D82:F82"/>
+    <mergeCell ref="D63:F63"/>
+    <mergeCell ref="D64:F64"/>
+    <mergeCell ref="D65:F65"/>
+    <mergeCell ref="D67:F67"/>
+    <mergeCell ref="D68:F68"/>
+    <mergeCell ref="D69:F69"/>
+    <mergeCell ref="D66:F66"/>
+    <mergeCell ref="D71:F71"/>
+    <mergeCell ref="D76:F76"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B27:C27"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B26:C26"/>
@@ -3473,74 +3483,160 @@
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="D101:F101"/>
-    <mergeCell ref="D106:F106"/>
-    <mergeCell ref="D111:F111"/>
-    <mergeCell ref="D116:F116"/>
-    <mergeCell ref="D98:F98"/>
-    <mergeCell ref="D99:F99"/>
-    <mergeCell ref="D100:F100"/>
-    <mergeCell ref="D102:F102"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="D50:F50"/>
+    <mergeCell ref="D51:F51"/>
+    <mergeCell ref="D52:F52"/>
+    <mergeCell ref="B171:C171"/>
+    <mergeCell ref="D171:F171"/>
+    <mergeCell ref="B172:C172"/>
+    <mergeCell ref="B173:C173"/>
+    <mergeCell ref="B174:C174"/>
+    <mergeCell ref="B175:C175"/>
+    <mergeCell ref="B176:C176"/>
+    <mergeCell ref="B177:C177"/>
+    <mergeCell ref="B178:C178"/>
+    <mergeCell ref="B179:C179"/>
+    <mergeCell ref="B180:C180"/>
+    <mergeCell ref="B181:C181"/>
+    <mergeCell ref="D172:F172"/>
+    <mergeCell ref="D173:F173"/>
+    <mergeCell ref="D174:F174"/>
+    <mergeCell ref="D175:F175"/>
+    <mergeCell ref="D176:F176"/>
+    <mergeCell ref="D177:F177"/>
+    <mergeCell ref="D178:F178"/>
+    <mergeCell ref="D179:F179"/>
+    <mergeCell ref="D180:F180"/>
+    <mergeCell ref="D181:F181"/>
+    <mergeCell ref="B163:C163"/>
+    <mergeCell ref="B164:C164"/>
+    <mergeCell ref="B165:C165"/>
+    <mergeCell ref="B166:C166"/>
+    <mergeCell ref="B167:C167"/>
+    <mergeCell ref="B168:C168"/>
+    <mergeCell ref="B169:C169"/>
+    <mergeCell ref="B170:C170"/>
+    <mergeCell ref="D163:F163"/>
+    <mergeCell ref="D164:F164"/>
+    <mergeCell ref="D165:F165"/>
+    <mergeCell ref="D166:F166"/>
+    <mergeCell ref="D167:F167"/>
+    <mergeCell ref="D168:F168"/>
+    <mergeCell ref="D169:F169"/>
+    <mergeCell ref="D170:F170"/>
+    <mergeCell ref="B162:C162"/>
+    <mergeCell ref="D162:F162"/>
+    <mergeCell ref="B158:C158"/>
+    <mergeCell ref="B159:C159"/>
+    <mergeCell ref="B160:C160"/>
+    <mergeCell ref="B161:C161"/>
+    <mergeCell ref="D158:F158"/>
+    <mergeCell ref="D159:F159"/>
+    <mergeCell ref="D160:F160"/>
+    <mergeCell ref="D161:F161"/>
+    <mergeCell ref="B157:C157"/>
+    <mergeCell ref="D157:F157"/>
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="D150:F150"/>
+    <mergeCell ref="B151:C151"/>
+    <mergeCell ref="B152:C152"/>
+    <mergeCell ref="B153:C153"/>
+    <mergeCell ref="B154:C154"/>
+    <mergeCell ref="B155:C155"/>
+    <mergeCell ref="B156:C156"/>
+    <mergeCell ref="D151:F151"/>
+    <mergeCell ref="D152:F152"/>
+    <mergeCell ref="D153:F153"/>
+    <mergeCell ref="D154:F154"/>
+    <mergeCell ref="D155:F155"/>
+    <mergeCell ref="D156:F156"/>
+    <mergeCell ref="D142:F142"/>
+    <mergeCell ref="D143:F143"/>
+    <mergeCell ref="D144:F144"/>
+    <mergeCell ref="D145:F145"/>
+    <mergeCell ref="D146:F146"/>
+    <mergeCell ref="D147:F147"/>
+    <mergeCell ref="D148:F148"/>
+    <mergeCell ref="D149:F149"/>
+    <mergeCell ref="B142:C142"/>
+    <mergeCell ref="B143:C143"/>
+    <mergeCell ref="B144:C144"/>
+    <mergeCell ref="B145:C145"/>
+    <mergeCell ref="B146:C146"/>
+    <mergeCell ref="B147:C147"/>
+    <mergeCell ref="B148:C148"/>
+    <mergeCell ref="B149:C149"/>
+    <mergeCell ref="B141:C141"/>
+    <mergeCell ref="D141:F141"/>
+    <mergeCell ref="B132:C132"/>
+    <mergeCell ref="D132:F132"/>
+    <mergeCell ref="D133:F133"/>
+    <mergeCell ref="D134:F134"/>
+    <mergeCell ref="D135:F135"/>
+    <mergeCell ref="D136:F136"/>
+    <mergeCell ref="D137:F137"/>
+    <mergeCell ref="D138:F138"/>
+    <mergeCell ref="D139:F139"/>
+    <mergeCell ref="D140:F140"/>
+    <mergeCell ref="B133:C133"/>
+    <mergeCell ref="B134:C134"/>
+    <mergeCell ref="B135:C135"/>
+    <mergeCell ref="B136:C136"/>
+    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="B138:C138"/>
+    <mergeCell ref="B139:C139"/>
+    <mergeCell ref="B140:C140"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="D126:F126"/>
+    <mergeCell ref="D127:F127"/>
+    <mergeCell ref="D128:F128"/>
+    <mergeCell ref="D129:F129"/>
+    <mergeCell ref="D130:F130"/>
+    <mergeCell ref="D131:F131"/>
+    <mergeCell ref="B124:C124"/>
+    <mergeCell ref="B125:C125"/>
+    <mergeCell ref="B126:C126"/>
+    <mergeCell ref="B127:C127"/>
+    <mergeCell ref="B128:C128"/>
+    <mergeCell ref="B129:C129"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="B131:C131"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="B117:C117"/>
+    <mergeCell ref="B118:C118"/>
+    <mergeCell ref="B119:C119"/>
+    <mergeCell ref="B120:C120"/>
+    <mergeCell ref="B121:C121"/>
+    <mergeCell ref="B122:C122"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="D61:F61"/>
     <mergeCell ref="B60:C60"/>
     <mergeCell ref="B62:C62"/>
     <mergeCell ref="B63:C63"/>
@@ -3555,98 +3651,6 @@
     <mergeCell ref="B56:C56"/>
     <mergeCell ref="B75:C75"/>
     <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B93:C93"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D40:F40"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="D60:F60"/>
-    <mergeCell ref="D57:F57"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="D59:F59"/>
-    <mergeCell ref="D62:F62"/>
-    <mergeCell ref="D53:F53"/>
-    <mergeCell ref="D54:F54"/>
-    <mergeCell ref="D55:F55"/>
-    <mergeCell ref="D75:F75"/>
-    <mergeCell ref="D77:F77"/>
-    <mergeCell ref="D78:F78"/>
-    <mergeCell ref="D79:F79"/>
-    <mergeCell ref="D80:F80"/>
-    <mergeCell ref="D82:F82"/>
-    <mergeCell ref="D63:F63"/>
-    <mergeCell ref="D64:F64"/>
-    <mergeCell ref="D65:F65"/>
-    <mergeCell ref="D67:F67"/>
-    <mergeCell ref="D68:F68"/>
-    <mergeCell ref="D69:F69"/>
-    <mergeCell ref="D66:F66"/>
-    <mergeCell ref="D71:F71"/>
-    <mergeCell ref="D76:F76"/>
-    <mergeCell ref="D81:F81"/>
-    <mergeCell ref="D70:F70"/>
-    <mergeCell ref="D72:F72"/>
-    <mergeCell ref="D73:F73"/>
-    <mergeCell ref="D74:F74"/>
-    <mergeCell ref="D90:F90"/>
-    <mergeCell ref="D92:F92"/>
-    <mergeCell ref="D93:F93"/>
-    <mergeCell ref="D94:F94"/>
-    <mergeCell ref="D95:F95"/>
-    <mergeCell ref="D97:F97"/>
-    <mergeCell ref="D83:F83"/>
-    <mergeCell ref="D84:F84"/>
-    <mergeCell ref="D85:F85"/>
-    <mergeCell ref="D87:F87"/>
-    <mergeCell ref="D88:F88"/>
-    <mergeCell ref="D89:F89"/>
-    <mergeCell ref="D96:F96"/>
-    <mergeCell ref="D86:F86"/>
-    <mergeCell ref="D91:F91"/>
-    <mergeCell ref="D110:F110"/>
-    <mergeCell ref="D112:F112"/>
-    <mergeCell ref="D103:F103"/>
-    <mergeCell ref="D104:F104"/>
-    <mergeCell ref="D105:F105"/>
-    <mergeCell ref="D107:F107"/>
-    <mergeCell ref="D108:F108"/>
-    <mergeCell ref="D109:F109"/>
-    <mergeCell ref="D120:F120"/>
-    <mergeCell ref="D122:F122"/>
-    <mergeCell ref="D123:F123"/>
-    <mergeCell ref="D124:F124"/>
-    <mergeCell ref="D125:F125"/>
-    <mergeCell ref="D113:F113"/>
-    <mergeCell ref="D114:F114"/>
-    <mergeCell ref="D115:F115"/>
-    <mergeCell ref="D117:F117"/>
-    <mergeCell ref="D118:F118"/>
-    <mergeCell ref="D119:F119"/>
-    <mergeCell ref="D121:F121"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update in measurements document
</commit_message>
<xml_diff>
--- a/doc/Sprint_1/1222123/Measurements_Building2.xlsx
+++ b/doc/Sprint_1/1222123/Measurements_Building2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr codeName="EsteLivro" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\Desktop\rcomp-dg-g1\doc\Sprint_1\1222123\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sousa\IdeaProjects\rcomp-dg-g1\doc\Sprint_1\1222123\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0F7981-A15F-4906-9252-663B25DC0C44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C793CDD0-FDFC-49EA-BC85-C62AE6FF6E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{933D9862-C879-4DBF-8626-28FC115C8F48}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{933D9862-C879-4DBF-8626-28FC115C8F48}"/>
   </bookViews>
   <sheets>
     <sheet name="Cable Measurements" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="104">
   <si>
     <t>Rooms</t>
   </si>
@@ -344,6 +344,12 @@
   </si>
   <si>
     <t>Distance in meters to CP in 2.1.15</t>
+  </si>
+  <si>
+    <t>Standart Height of CP already included on Measurements</t>
+  </si>
+  <si>
+    <t>1,7m</t>
   </si>
 </sst>
 </file>
@@ -394,7 +400,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -454,15 +460,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -470,6 +523,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
@@ -486,8 +548,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Verificar Célula" xfId="1" builtinId="23"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -503,7 +565,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -822,8 +884,8 @@
   <sheetPr codeName="Folha1"/>
   <dimension ref="B1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14:J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,61 +896,61 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="G2" s="3" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="G2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="M2" s="3" t="s">
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="M2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
     </row>
     <row r="3" spans="2:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="4"/>
       <c r="D3" s="1"/>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="M3" s="3" t="s">
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="M3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
     </row>
     <row r="4" spans="2:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="4"/>
       <c r="D4" s="1"/>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="M4" s="3" t="s">
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="M4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
     </row>
     <row r="5" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -902,12 +964,12 @@
       <c r="D9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
     </row>
     <row r="10" spans="2:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
@@ -925,10 +987,10 @@
       <c r="H10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J10" s="3"/>
+      <c r="J10" s="4"/>
     </row>
     <row r="11" spans="2:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
@@ -946,8 +1008,10 @@
       <c r="H11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="5"/>
+      <c r="I11" s="5">
+        <v>20</v>
+      </c>
+      <c r="J11" s="6"/>
     </row>
     <row r="12" spans="2:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
@@ -965,8 +1029,10 @@
       <c r="H12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="5"/>
+      <c r="I12" s="5">
+        <v>38</v>
+      </c>
+      <c r="J12" s="6"/>
     </row>
     <row r="13" spans="2:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
@@ -984,8 +1050,10 @@
       <c r="H13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I13" s="4"/>
-      <c r="J13" s="5"/>
+      <c r="I13" s="5">
+        <v>14.23</v>
+      </c>
+      <c r="J13" s="6"/>
     </row>
     <row r="14" spans="2:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
@@ -1003,8 +1071,10 @@
       <c r="H14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="5"/>
+      <c r="I14" s="5">
+        <v>39.04</v>
+      </c>
+      <c r="J14" s="6"/>
     </row>
     <row r="15" spans="2:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
@@ -1050,14 +1120,16 @@
       <c r="D18" s="1">
         <v>6</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="1"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="1">
+        <v>7.69</v>
+      </c>
     </row>
     <row r="19" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
@@ -1291,8 +1363,8 @@
   <sheetPr codeName="Folha2"/>
   <dimension ref="B2:L29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1302,331 +1374,435 @@
   <sheetData>
     <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="I3" s="3" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="I3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
     </row>
     <row r="4" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="I4" s="3" t="s">
+      <c r="F4" s="4"/>
+      <c r="I4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3" t="s">
+      <c r="J4" s="4"/>
+      <c r="K4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="L4" s="3"/>
+      <c r="L4" s="4"/>
     </row>
     <row r="5" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="I5" s="3" t="s">
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="I5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="4" t="s">
+      <c r="J5" s="4"/>
+      <c r="K5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="5"/>
+      <c r="L5" s="6"/>
     </row>
     <row r="6" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="I6" s="3" t="s">
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4">
+        <v>7</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="I6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="4" t="s">
+      <c r="J6" s="4"/>
+      <c r="K6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L6" s="5"/>
+      <c r="L6" s="6"/>
     </row>
     <row r="7" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="4" t="s">
+      <c r="J7" s="4"/>
+      <c r="K7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L7" s="5"/>
+      <c r="L7" s="6"/>
     </row>
     <row r="8" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="3"/>
-      <c r="K8" s="4" t="s">
+      <c r="J8" s="4"/>
+      <c r="K8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L8" s="5"/>
+      <c r="L8" s="6"/>
     </row>
     <row r="9" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="I9" s="3" t="s">
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="I9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="3"/>
-      <c r="K9" s="4" t="s">
+      <c r="J9" s="4"/>
+      <c r="K9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="5"/>
+      <c r="L9" s="6"/>
     </row>
     <row r="10" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="3" t="s">
+      <c r="C10" s="4"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="I10" s="3" t="s">
+      <c r="F10" s="4"/>
+      <c r="I10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="3"/>
-      <c r="K10" s="4" t="s">
+      <c r="J10" s="4"/>
+      <c r="K10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="L10" s="5"/>
+      <c r="L10" s="6"/>
     </row>
     <row r="11" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I11" s="3" t="s">
+      <c r="B11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="4">
+        <v>54.3</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="I11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="3"/>
-      <c r="K11" s="4" t="s">
+      <c r="J11" s="4"/>
+      <c r="K11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="L11" s="5"/>
+      <c r="L11" s="6"/>
     </row>
     <row r="12" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I12" s="3" t="s">
+      <c r="B12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="4">
+        <v>45.3</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="I12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="4" t="s">
+      <c r="J12" s="4"/>
+      <c r="K12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L12" s="5"/>
+      <c r="L12" s="6"/>
     </row>
     <row r="13" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I13" s="3" t="s">
+      <c r="B13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="4">
+        <v>22.88</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="I13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J13" s="3"/>
-      <c r="K13" s="4" t="s">
+      <c r="J13" s="4"/>
+      <c r="K13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L13" s="5"/>
+      <c r="L13" s="6"/>
     </row>
     <row r="14" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I14" s="3" t="s">
+      <c r="B14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="4">
+        <v>10</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="I14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J14" s="3"/>
-      <c r="K14" s="4" t="s">
+      <c r="J14" s="4"/>
+      <c r="K14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L14" s="5"/>
+      <c r="L14" s="6"/>
     </row>
     <row r="15" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="I15" s="3" t="s">
+      <c r="I15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J15" s="3"/>
-      <c r="K15" s="4" t="s">
+      <c r="J15" s="4"/>
+      <c r="K15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L15" s="5"/>
+      <c r="L15" s="6"/>
     </row>
     <row r="16" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="I16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="4"/>
+      <c r="K16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L16" s="6"/>
+    </row>
+    <row r="17" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="3" t="s">
+      <c r="C17" s="4"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="I16" s="3" t="s">
+      <c r="F17" s="4"/>
+      <c r="I17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" s="4"/>
+      <c r="K17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="4" t="s">
+      <c r="L17" s="6"/>
+    </row>
+    <row r="18" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L16" s="5"/>
-    </row>
-    <row r="17" spans="9:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J17" s="3"/>
-      <c r="K17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="L17" s="5"/>
-    </row>
-    <row r="18" spans="9:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I18" s="3" t="s">
+      <c r="C18" s="6"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="5">
+        <v>57.17</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="I18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J18" s="3"/>
-      <c r="K18" s="4" t="s">
+      <c r="J18" s="4"/>
+      <c r="K18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="L18" s="5"/>
-    </row>
-    <row r="19" spans="9:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="3" t="s">
+      <c r="L18" s="6"/>
+    </row>
+    <row r="19" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="5">
+        <v>44.1</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="I19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J19" s="3"/>
-      <c r="K19" s="4" t="s">
+      <c r="J19" s="4"/>
+      <c r="K19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="L19" s="5"/>
-    </row>
-    <row r="20" spans="9:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I20" s="3" t="s">
+      <c r="L19" s="6"/>
+    </row>
+    <row r="20" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="5">
+        <v>21.6</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="I20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J20" s="3"/>
-      <c r="K20" s="4" t="s">
+      <c r="J20" s="4"/>
+      <c r="K20" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L20" s="5"/>
-    </row>
-    <row r="21" spans="9:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="3" t="s">
+      <c r="L20" s="6"/>
+    </row>
+    <row r="21" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="5">
+        <v>16.02</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="I21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="3"/>
-      <c r="K21" s="4" t="s">
+      <c r="J21" s="4"/>
+      <c r="K21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L21" s="5"/>
-    </row>
-    <row r="22" spans="9:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I22" s="3" t="s">
+      <c r="L21" s="6"/>
+    </row>
+    <row r="22" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="5">
+        <v>6.6</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="I22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J22" s="3"/>
-      <c r="K22" s="4" t="s">
+      <c r="J22" s="4"/>
+      <c r="K22" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L22" s="5"/>
-    </row>
-    <row r="23" spans="9:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I23" s="3" t="s">
+      <c r="L22" s="6"/>
+    </row>
+    <row r="23" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="6"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="5">
+        <v>54.97</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="I23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J23" s="3"/>
-      <c r="K23" s="4" t="s">
+      <c r="J23" s="4"/>
+      <c r="K23" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L23" s="5"/>
-    </row>
-    <row r="24" spans="9:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="3" t="s">
+      <c r="L23" s="6"/>
+    </row>
+    <row r="24" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="5">
+        <v>58.82</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="I24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J24" s="3"/>
-      <c r="K24" s="4" t="s">
+      <c r="J24" s="4"/>
+      <c r="K24" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L24" s="5"/>
-    </row>
-    <row r="25" spans="9:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I25" s="3" t="s">
+      <c r="L24" s="6"/>
+    </row>
+    <row r="25" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I25" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="J25" s="3"/>
-      <c r="K25" s="4" t="s">
+      <c r="J25" s="4"/>
+      <c r="K25" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L25" s="5"/>
-    </row>
-    <row r="26" spans="9:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I26" s="3" t="s">
+      <c r="L25" s="6"/>
+    </row>
+    <row r="26" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I26" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J26" s="3"/>
-      <c r="K26" s="4" t="s">
+      <c r="J26" s="4"/>
+      <c r="K26" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="L26" s="5"/>
-    </row>
-    <row r="27" spans="9:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="3" t="s">
+      <c r="L26" s="6"/>
+    </row>
+    <row r="27" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I27" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J27" s="3"/>
-      <c r="K27" s="4" t="s">
+      <c r="J27" s="4"/>
+      <c r="K27" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="L27" s="5"/>
-    </row>
-    <row r="28" spans="9:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I28" s="3" t="s">
+      <c r="L27" s="6"/>
+    </row>
+    <row r="28" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I28" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J28" s="3"/>
-      <c r="K28" s="4" t="s">
+      <c r="J28" s="4"/>
+      <c r="K28" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="L28" s="5"/>
-    </row>
-    <row r="29" spans="9:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="L28" s="6"/>
+    </row>
+    <row r="29" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="65">
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="E16:F16"/>
+  <mergeCells count="89">
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="E4:F4"/>
@@ -1640,20 +1816,18 @@
     <mergeCell ref="B9:F9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="E10:F10"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
     <mergeCell ref="I3:L3"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="I17:J17"/>
@@ -1661,34 +1835,63 @@
     <mergeCell ref="I19:J19"/>
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="I21:J21"/>
-    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="I24:J24"/>
     <mergeCell ref="I25:J25"/>
     <mergeCell ref="I26:J26"/>
     <mergeCell ref="I27:J27"/>
     <mergeCell ref="K23:L23"/>
     <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K15:L15"/>
     <mergeCell ref="I14:J14"/>
     <mergeCell ref="I15:J15"/>
     <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K14:L14"/>
     <mergeCell ref="K28:L28"/>
     <mergeCell ref="K27:L27"/>
     <mergeCell ref="K26:L26"/>
     <mergeCell ref="K25:L25"/>
     <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D10:D14"/>
+    <mergeCell ref="D17:D24"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1700,8 +1903,8 @@
   <sheetPr codeName="Folha3"/>
   <dimension ref="B1:H182"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D171" sqref="D171:F171"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1724,8 +1927,20 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>50</v>
@@ -1736,1637 +1951,1753 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="2:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
+      <c r="C6" s="4"/>
+      <c r="D6" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="2:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="2:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4">
+        <v>13.94</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="2:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4">
+        <v>11.05</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="2:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4">
+        <v>20.21</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="2:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4">
+        <v>16.940000000000001</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
     </row>
     <row r="12" spans="2:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4">
+        <v>14.05</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="2:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3" t="s">
+      <c r="C13" s="4"/>
+      <c r="D13" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="2:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4">
+        <v>13.55</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
     </row>
     <row r="15" spans="2:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="5">
+        <v>10.28</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" spans="2:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="5">
+        <v>7.4</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="5">
+        <v>16.850000000000001</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="5">
+        <v>13.58</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="5">
+        <v>10.7</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="6"/>
     </row>
     <row r="20" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="4" t="s">
+      <c r="C20" s="6"/>
+      <c r="D20" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="5"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="5">
+        <v>6.63</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="5">
+        <v>3.94</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" s="6"/>
     </row>
     <row r="23" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="5">
+        <v>9.93</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="6"/>
     </row>
     <row r="24" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="5"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="5">
+        <v>7.24</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" s="6"/>
     </row>
     <row r="25" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="4" t="s">
+      <c r="C25" s="6"/>
+      <c r="D25" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="E25" s="6"/>
-      <c r="F25" s="5"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="6"/>
     </row>
     <row r="26" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="5"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="5">
+        <v>15.28</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="F26" s="6"/>
     </row>
     <row r="27" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="5"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="5">
+        <v>12.59</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="F27" s="6"/>
     </row>
     <row r="28" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="5"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="5">
+        <v>18.579999999999998</v>
+      </c>
+      <c r="E28" s="10"/>
+      <c r="F28" s="6"/>
     </row>
     <row r="29" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="5"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="5">
+        <v>15.89</v>
+      </c>
+      <c r="E29" s="10"/>
+      <c r="F29" s="6"/>
     </row>
     <row r="30" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="4" t="s">
+      <c r="C30" s="6"/>
+      <c r="D30" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="5"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="6"/>
     </row>
     <row r="31" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="5"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="5">
+        <v>13.24</v>
+      </c>
+      <c r="E31" s="10"/>
+      <c r="F31" s="6"/>
     </row>
     <row r="32" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="5"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="5">
+        <v>11.78</v>
+      </c>
+      <c r="E32" s="10"/>
+      <c r="F32" s="6"/>
     </row>
     <row r="33" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="5"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="5">
+        <v>10.32</v>
+      </c>
+      <c r="E33" s="10"/>
+      <c r="F33" s="6"/>
     </row>
     <row r="34" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="5"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="5">
+        <v>8.86</v>
+      </c>
+      <c r="E34" s="10"/>
+      <c r="F34" s="6"/>
     </row>
     <row r="35" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="5"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="5">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E35" s="10"/>
+      <c r="F35" s="6"/>
     </row>
     <row r="36" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="5"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="5">
+        <v>16.32</v>
+      </c>
+      <c r="E36" s="10"/>
+      <c r="F36" s="6"/>
     </row>
     <row r="37" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="5"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="5">
+        <v>14.66</v>
+      </c>
+      <c r="E37" s="10"/>
+      <c r="F37" s="6"/>
     </row>
     <row r="38" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="5"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="5">
+        <v>11.18</v>
+      </c>
+      <c r="E38" s="10"/>
+      <c r="F38" s="6"/>
     </row>
     <row r="39" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="5"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="5">
+        <v>9.41</v>
+      </c>
+      <c r="E39" s="10"/>
+      <c r="F39" s="6"/>
     </row>
     <row r="40" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C40" s="5"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="5"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="5">
+        <v>7.64</v>
+      </c>
+      <c r="E40" s="10"/>
+      <c r="F40" s="6"/>
     </row>
     <row r="41" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="5"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="5">
+        <v>5.87</v>
+      </c>
+      <c r="E41" s="10"/>
+      <c r="F41" s="6"/>
     </row>
     <row r="42" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="5"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="5">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E42" s="10"/>
+      <c r="F42" s="6"/>
     </row>
     <row r="43" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="4" t="s">
+      <c r="C43" s="6"/>
+      <c r="D43" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E43" s="6"/>
-      <c r="F43" s="5"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="6"/>
     </row>
     <row r="44" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C44" s="5"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="5"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="5">
+        <v>11.9</v>
+      </c>
+      <c r="E44" s="10"/>
+      <c r="F44" s="6"/>
     </row>
     <row r="45" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="5"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="5">
+        <v>8.17</v>
+      </c>
+      <c r="E45" s="10"/>
+      <c r="F45" s="6"/>
     </row>
     <row r="46" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="5"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="5">
+        <v>6.63</v>
+      </c>
+      <c r="E46" s="10"/>
+      <c r="F46" s="6"/>
     </row>
     <row r="47" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="5"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="5">
+        <v>4.71</v>
+      </c>
+      <c r="E47" s="10"/>
+      <c r="F47" s="6"/>
     </row>
     <row r="48" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="5"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="5">
+        <v>3.4</v>
+      </c>
+      <c r="E48" s="10"/>
+      <c r="F48" s="6"/>
     </row>
     <row r="49" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C49" s="5"/>
-      <c r="D49" s="4" t="s">
+      <c r="C49" s="6"/>
+      <c r="D49" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E49" s="6"/>
-      <c r="F49" s="5"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="6"/>
     </row>
     <row r="50" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C50" s="5"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="5"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="5">
+        <v>12.02</v>
+      </c>
+      <c r="E50" s="10"/>
+      <c r="F50" s="6"/>
     </row>
     <row r="51" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C51" s="5"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="9"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="11">
+        <v>8.5500000000000007</v>
+      </c>
+      <c r="E51" s="12"/>
+      <c r="F51" s="13"/>
     </row>
     <row r="52" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C52" s="5"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="5"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="5">
+        <v>6.82</v>
+      </c>
+      <c r="E52" s="10"/>
+      <c r="F52" s="6"/>
     </row>
     <row r="53" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C53" s="5"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="5"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="5">
+        <v>5.09</v>
+      </c>
+      <c r="E53" s="10"/>
+      <c r="F53" s="6"/>
     </row>
     <row r="54" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C54" s="5"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="5"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="5">
+        <v>3.94</v>
+      </c>
+      <c r="E54" s="10"/>
+      <c r="F54" s="6"/>
     </row>
     <row r="55" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C55" s="5"/>
-      <c r="D55" s="4" t="s">
+      <c r="C55" s="6"/>
+      <c r="D55" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="E55" s="6"/>
-      <c r="F55" s="5"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="6"/>
     </row>
     <row r="56" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C56" s="5"/>
-      <c r="D56" s="4"/>
-      <c r="E56" s="6"/>
-      <c r="F56" s="5"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="5">
+        <v>12.98</v>
+      </c>
+      <c r="E56" s="10"/>
+      <c r="F56" s="6"/>
     </row>
     <row r="57" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C57" s="5"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="5"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="5">
+        <v>10.28</v>
+      </c>
+      <c r="E57" s="10"/>
+      <c r="F57" s="6"/>
     </row>
     <row r="58" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C58" s="5"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="5"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="5">
+        <v>7.78</v>
+      </c>
+      <c r="E58" s="10"/>
+      <c r="F58" s="6"/>
     </row>
     <row r="59" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C59" s="5"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="6"/>
-      <c r="F59" s="5"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="5">
+        <v>16.28</v>
+      </c>
+      <c r="E59" s="10"/>
+      <c r="F59" s="6"/>
     </row>
     <row r="60" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C60" s="5"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="6"/>
-      <c r="F60" s="5"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="5">
+        <v>13.58</v>
+      </c>
+      <c r="E60" s="10"/>
+      <c r="F60" s="6"/>
     </row>
     <row r="61" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C61" s="5"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="6"/>
-      <c r="F61" s="5"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="5">
+        <v>11.08</v>
+      </c>
+      <c r="E61" s="10"/>
+      <c r="F61" s="6"/>
     </row>
     <row r="62" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C62" s="5"/>
-      <c r="D62" s="4" t="s">
+      <c r="C62" s="6"/>
+      <c r="D62" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="E62" s="6"/>
-      <c r="F62" s="5"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="6"/>
     </row>
     <row r="63" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C63" s="5"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="6"/>
-      <c r="F63" s="5"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="5">
+        <v>9.32</v>
+      </c>
+      <c r="E63" s="10"/>
+      <c r="F63" s="6"/>
     </row>
     <row r="64" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C64" s="5"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="6"/>
-      <c r="F64" s="5"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="5">
+        <v>6.63</v>
+      </c>
+      <c r="E64" s="10"/>
+      <c r="F64" s="6"/>
     </row>
     <row r="65" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C65" s="5"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="6"/>
-      <c r="F65" s="5"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="5">
+        <v>4.13</v>
+      </c>
+      <c r="E65" s="10"/>
+      <c r="F65" s="6"/>
     </row>
     <row r="66" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C66" s="5"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="6"/>
-      <c r="F66" s="5"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="5">
+        <v>12.62</v>
+      </c>
+      <c r="E66" s="10"/>
+      <c r="F66" s="6"/>
     </row>
     <row r="67" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C67" s="5"/>
-      <c r="D67" s="4"/>
-      <c r="E67" s="6"/>
-      <c r="F67" s="5"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="5">
+        <v>9.93</v>
+      </c>
+      <c r="E67" s="10"/>
+      <c r="F67" s="6"/>
     </row>
     <row r="68" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C68" s="5"/>
-      <c r="D68" s="4"/>
-      <c r="E68" s="6"/>
-      <c r="F68" s="5"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="5">
+        <v>7.43</v>
+      </c>
+      <c r="E68" s="10"/>
+      <c r="F68" s="6"/>
     </row>
     <row r="69" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C69" s="5"/>
-      <c r="D69" s="4" t="s">
+      <c r="C69" s="6"/>
+      <c r="D69" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="E69" s="6"/>
-      <c r="F69" s="5"/>
+      <c r="E69" s="10"/>
+      <c r="F69" s="6"/>
     </row>
     <row r="70" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C70" s="5"/>
-      <c r="D70" s="4"/>
-      <c r="E70" s="6"/>
-      <c r="F70" s="5"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="5">
+        <v>23.4</v>
+      </c>
+      <c r="E70" s="10"/>
+      <c r="F70" s="6"/>
     </row>
     <row r="71" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C71" s="5"/>
-      <c r="D71" s="4"/>
-      <c r="E71" s="6"/>
-      <c r="F71" s="5"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="5">
+        <v>20.75</v>
+      </c>
+      <c r="E71" s="10"/>
+      <c r="F71" s="6"/>
     </row>
     <row r="72" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C72" s="5"/>
-      <c r="D72" s="4"/>
-      <c r="E72" s="6"/>
-      <c r="F72" s="5"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="5">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="E72" s="10"/>
+      <c r="F72" s="6"/>
     </row>
     <row r="73" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C73" s="5"/>
-      <c r="D73" s="4"/>
-      <c r="E73" s="6"/>
-      <c r="F73" s="5"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="5">
+        <v>17.45</v>
+      </c>
+      <c r="E73" s="10"/>
+      <c r="F73" s="6"/>
     </row>
     <row r="74" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C74" s="5"/>
-      <c r="D74" s="4" t="s">
+      <c r="C74" s="6"/>
+      <c r="D74" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="E74" s="6"/>
-      <c r="F74" s="5"/>
+      <c r="E74" s="10"/>
+      <c r="F74" s="6"/>
     </row>
     <row r="75" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="4" t="s">
+      <c r="B75" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C75" s="5"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="6"/>
-      <c r="F75" s="5"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="10"/>
+      <c r="F75" s="6"/>
     </row>
     <row r="76" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="4" t="s">
+      <c r="B76" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C76" s="5"/>
-      <c r="D76" s="4"/>
-      <c r="E76" s="6"/>
-      <c r="F76" s="5"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="10"/>
+      <c r="F76" s="6"/>
     </row>
     <row r="77" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="4" t="s">
+      <c r="B77" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C77" s="5"/>
-      <c r="D77" s="4"/>
-      <c r="E77" s="6"/>
-      <c r="F77" s="5"/>
+      <c r="C77" s="6"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="10"/>
+      <c r="F77" s="6"/>
     </row>
     <row r="78" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="4" t="s">
+      <c r="B78" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C78" s="5"/>
-      <c r="D78" s="4"/>
-      <c r="E78" s="6"/>
-      <c r="F78" s="5"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="10"/>
+      <c r="F78" s="6"/>
     </row>
     <row r="79" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="4" t="s">
+      <c r="B79" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C79" s="5"/>
-      <c r="D79" s="4"/>
-      <c r="E79" s="6"/>
-      <c r="F79" s="5"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="10"/>
+      <c r="F79" s="6"/>
     </row>
     <row r="80" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="4" t="s">
+      <c r="B80" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C80" s="5"/>
-      <c r="D80" s="4"/>
-      <c r="E80" s="6"/>
-      <c r="F80" s="5"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="10"/>
+      <c r="F80" s="6"/>
     </row>
     <row r="81" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="4" t="s">
+      <c r="B81" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C81" s="5"/>
-      <c r="D81" s="4" t="s">
+      <c r="C81" s="6"/>
+      <c r="D81" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="E81" s="6"/>
-      <c r="F81" s="5"/>
+      <c r="E81" s="10"/>
+      <c r="F81" s="6"/>
     </row>
     <row r="82" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="4" t="s">
+      <c r="B82" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C82" s="5"/>
-      <c r="D82" s="4"/>
-      <c r="E82" s="6"/>
-      <c r="F82" s="5"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="10"/>
+      <c r="F82" s="6"/>
     </row>
     <row r="83" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="4" t="s">
+      <c r="B83" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C83" s="5"/>
-      <c r="D83" s="4"/>
-      <c r="E83" s="6"/>
-      <c r="F83" s="5"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="5"/>
+      <c r="E83" s="10"/>
+      <c r="F83" s="6"/>
     </row>
     <row r="84" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="4" t="s">
+      <c r="B84" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C84" s="5"/>
-      <c r="D84" s="4"/>
-      <c r="E84" s="6"/>
-      <c r="F84" s="5"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="10"/>
+      <c r="F84" s="6"/>
     </row>
     <row r="85" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="4" t="s">
+      <c r="B85" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C85" s="5"/>
-      <c r="D85" s="4"/>
-      <c r="E85" s="6"/>
-      <c r="F85" s="5"/>
+      <c r="C85" s="6"/>
+      <c r="D85" s="5"/>
+      <c r="E85" s="10"/>
+      <c r="F85" s="6"/>
     </row>
     <row r="86" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="4" t="s">
+      <c r="B86" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C86" s="5"/>
-      <c r="D86" s="4"/>
-      <c r="E86" s="6"/>
-      <c r="F86" s="5"/>
+      <c r="C86" s="6"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="10"/>
+      <c r="F86" s="6"/>
     </row>
     <row r="87" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="4" t="s">
+      <c r="B87" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C87" s="5"/>
-      <c r="D87" s="4"/>
-      <c r="E87" s="6"/>
-      <c r="F87" s="5"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="5"/>
+      <c r="E87" s="10"/>
+      <c r="F87" s="6"/>
     </row>
     <row r="88" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="4" t="s">
+      <c r="B88" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C88" s="5"/>
-      <c r="D88" s="4" t="s">
+      <c r="C88" s="6"/>
+      <c r="D88" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="E88" s="6"/>
-      <c r="F88" s="5"/>
+      <c r="E88" s="10"/>
+      <c r="F88" s="6"/>
     </row>
     <row r="89" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="4" t="s">
+      <c r="B89" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C89" s="5"/>
-      <c r="D89" s="4"/>
-      <c r="E89" s="6"/>
-      <c r="F89" s="5"/>
+      <c r="C89" s="6"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="10"/>
+      <c r="F89" s="6"/>
     </row>
     <row r="90" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="4" t="s">
+      <c r="B90" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C90" s="5"/>
-      <c r="D90" s="4"/>
-      <c r="E90" s="6"/>
-      <c r="F90" s="5"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="5"/>
+      <c r="E90" s="10"/>
+      <c r="F90" s="6"/>
     </row>
     <row r="91" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="4" t="s">
+      <c r="B91" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C91" s="5"/>
-      <c r="D91" s="4"/>
-      <c r="E91" s="6"/>
-      <c r="F91" s="5"/>
+      <c r="C91" s="6"/>
+      <c r="D91" s="5"/>
+      <c r="E91" s="10"/>
+      <c r="F91" s="6"/>
     </row>
     <row r="92" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="4" t="s">
+      <c r="B92" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C92" s="5"/>
-      <c r="D92" s="4"/>
-      <c r="E92" s="6"/>
-      <c r="F92" s="5"/>
+      <c r="C92" s="6"/>
+      <c r="D92" s="5"/>
+      <c r="E92" s="10"/>
+      <c r="F92" s="6"/>
     </row>
     <row r="93" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="4" t="s">
+      <c r="B93" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C93" s="5"/>
-      <c r="D93" s="4"/>
-      <c r="E93" s="6"/>
-      <c r="F93" s="5"/>
+      <c r="C93" s="6"/>
+      <c r="D93" s="5"/>
+      <c r="E93" s="10"/>
+      <c r="F93" s="6"/>
     </row>
     <row r="94" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="4" t="s">
+      <c r="B94" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C94" s="5"/>
-      <c r="D94" s="4"/>
-      <c r="E94" s="6"/>
-      <c r="F94" s="5"/>
+      <c r="C94" s="6"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="10"/>
+      <c r="F94" s="6"/>
     </row>
     <row r="95" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="4" t="s">
+      <c r="B95" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C95" s="5"/>
-      <c r="D95" s="4" t="s">
+      <c r="C95" s="6"/>
+      <c r="D95" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="E95" s="6"/>
-      <c r="F95" s="5"/>
+      <c r="E95" s="10"/>
+      <c r="F95" s="6"/>
     </row>
     <row r="96" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="4" t="s">
+      <c r="B96" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C96" s="5"/>
-      <c r="D96" s="4"/>
-      <c r="E96" s="6"/>
-      <c r="F96" s="5"/>
+      <c r="C96" s="6"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="10"/>
+      <c r="F96" s="6"/>
     </row>
     <row r="97" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="4" t="s">
+      <c r="B97" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C97" s="5"/>
-      <c r="D97" s="4"/>
-      <c r="E97" s="6"/>
-      <c r="F97" s="5"/>
+      <c r="C97" s="6"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="10"/>
+      <c r="F97" s="6"/>
     </row>
     <row r="98" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="4" t="s">
+      <c r="B98" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C98" s="5"/>
-      <c r="D98" s="4"/>
-      <c r="E98" s="6"/>
-      <c r="F98" s="5"/>
+      <c r="C98" s="6"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="10"/>
+      <c r="F98" s="6"/>
     </row>
     <row r="99" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="4" t="s">
+      <c r="B99" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C99" s="5"/>
-      <c r="D99" s="4"/>
-      <c r="E99" s="6"/>
-      <c r="F99" s="5"/>
+      <c r="C99" s="6"/>
+      <c r="D99" s="5"/>
+      <c r="E99" s="10"/>
+      <c r="F99" s="6"/>
     </row>
     <row r="100" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="4" t="s">
+      <c r="B100" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C100" s="5"/>
-      <c r="D100" s="4"/>
-      <c r="E100" s="6"/>
-      <c r="F100" s="5"/>
+      <c r="C100" s="6"/>
+      <c r="D100" s="5"/>
+      <c r="E100" s="10"/>
+      <c r="F100" s="6"/>
     </row>
     <row r="101" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="4" t="s">
+      <c r="B101" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C101" s="5"/>
-      <c r="D101" s="4"/>
-      <c r="E101" s="6"/>
-      <c r="F101" s="5"/>
+      <c r="C101" s="6"/>
+      <c r="D101" s="5"/>
+      <c r="E101" s="10"/>
+      <c r="F101" s="6"/>
     </row>
     <row r="102" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="4" t="s">
+      <c r="B102" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C102" s="5"/>
-      <c r="D102" s="4" t="s">
+      <c r="C102" s="6"/>
+      <c r="D102" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="E102" s="6"/>
-      <c r="F102" s="5"/>
+      <c r="E102" s="10"/>
+      <c r="F102" s="6"/>
     </row>
     <row r="103" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="4" t="s">
+      <c r="B103" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C103" s="5"/>
-      <c r="D103" s="4"/>
-      <c r="E103" s="6"/>
-      <c r="F103" s="5"/>
+      <c r="C103" s="6"/>
+      <c r="D103" s="5"/>
+      <c r="E103" s="10"/>
+      <c r="F103" s="6"/>
     </row>
     <row r="104" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="4" t="s">
+      <c r="B104" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C104" s="5"/>
-      <c r="D104" s="4"/>
-      <c r="E104" s="6"/>
-      <c r="F104" s="5"/>
+      <c r="C104" s="6"/>
+      <c r="D104" s="5"/>
+      <c r="E104" s="10"/>
+      <c r="F104" s="6"/>
     </row>
     <row r="105" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="4" t="s">
+      <c r="B105" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C105" s="5"/>
-      <c r="D105" s="4"/>
-      <c r="E105" s="6"/>
-      <c r="F105" s="5"/>
+      <c r="C105" s="6"/>
+      <c r="D105" s="5"/>
+      <c r="E105" s="10"/>
+      <c r="F105" s="6"/>
     </row>
     <row r="106" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="4" t="s">
+      <c r="B106" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C106" s="5"/>
-      <c r="D106" s="4"/>
-      <c r="E106" s="6"/>
-      <c r="F106" s="5"/>
+      <c r="C106" s="6"/>
+      <c r="D106" s="5"/>
+      <c r="E106" s="10"/>
+      <c r="F106" s="6"/>
     </row>
     <row r="107" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B107" s="4" t="s">
+      <c r="B107" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C107" s="5"/>
-      <c r="D107" s="4"/>
-      <c r="E107" s="6"/>
-      <c r="F107" s="5"/>
+      <c r="C107" s="6"/>
+      <c r="D107" s="5"/>
+      <c r="E107" s="10"/>
+      <c r="F107" s="6"/>
     </row>
     <row r="108" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="4" t="s">
+      <c r="B108" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C108" s="5"/>
-      <c r="D108" s="4"/>
-      <c r="E108" s="6"/>
-      <c r="F108" s="5"/>
+      <c r="C108" s="6"/>
+      <c r="D108" s="5"/>
+      <c r="E108" s="10"/>
+      <c r="F108" s="6"/>
     </row>
     <row r="109" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="4" t="s">
+      <c r="B109" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C109" s="5"/>
-      <c r="D109" s="4" t="s">
+      <c r="C109" s="6"/>
+      <c r="D109" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E109" s="6"/>
-      <c r="F109" s="5"/>
+      <c r="E109" s="10"/>
+      <c r="F109" s="6"/>
     </row>
     <row r="110" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B110" s="4" t="s">
+      <c r="B110" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C110" s="5"/>
-      <c r="D110" s="4"/>
-      <c r="E110" s="6"/>
-      <c r="F110" s="5"/>
+      <c r="C110" s="6"/>
+      <c r="D110" s="5"/>
+      <c r="E110" s="10"/>
+      <c r="F110" s="6"/>
     </row>
     <row r="111" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="4" t="s">
+      <c r="B111" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C111" s="5"/>
-      <c r="D111" s="4"/>
-      <c r="E111" s="6"/>
-      <c r="F111" s="5"/>
+      <c r="C111" s="6"/>
+      <c r="D111" s="5"/>
+      <c r="E111" s="10"/>
+      <c r="F111" s="6"/>
     </row>
     <row r="112" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B112" s="4" t="s">
+      <c r="B112" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C112" s="5"/>
-      <c r="D112" s="4"/>
-      <c r="E112" s="6"/>
-      <c r="F112" s="5"/>
+      <c r="C112" s="6"/>
+      <c r="D112" s="5"/>
+      <c r="E112" s="10"/>
+      <c r="F112" s="6"/>
     </row>
     <row r="113" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="4" t="s">
+      <c r="B113" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C113" s="5"/>
-      <c r="D113" s="4"/>
-      <c r="E113" s="6"/>
-      <c r="F113" s="5"/>
+      <c r="C113" s="6"/>
+      <c r="D113" s="5"/>
+      <c r="E113" s="10"/>
+      <c r="F113" s="6"/>
     </row>
     <row r="114" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="4" t="s">
+      <c r="B114" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C114" s="5"/>
-      <c r="D114" s="4" t="s">
+      <c r="C114" s="6"/>
+      <c r="D114" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E114" s="6"/>
-      <c r="F114" s="5"/>
+      <c r="E114" s="10"/>
+      <c r="F114" s="6"/>
     </row>
     <row r="115" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B115" s="4" t="s">
+      <c r="B115" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C115" s="5"/>
-      <c r="D115" s="4"/>
-      <c r="E115" s="6"/>
-      <c r="F115" s="5"/>
+      <c r="C115" s="6"/>
+      <c r="D115" s="5"/>
+      <c r="E115" s="10"/>
+      <c r="F115" s="6"/>
     </row>
     <row r="116" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B116" s="4" t="s">
+      <c r="B116" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C116" s="5"/>
-      <c r="D116" s="4"/>
-      <c r="E116" s="6"/>
-      <c r="F116" s="5"/>
+      <c r="C116" s="6"/>
+      <c r="D116" s="5"/>
+      <c r="E116" s="10"/>
+      <c r="F116" s="6"/>
     </row>
     <row r="117" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B117" s="4" t="s">
+      <c r="B117" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C117" s="5"/>
-      <c r="D117" s="4"/>
-      <c r="E117" s="6"/>
-      <c r="F117" s="5"/>
+      <c r="C117" s="6"/>
+      <c r="D117" s="5"/>
+      <c r="E117" s="10"/>
+      <c r="F117" s="6"/>
     </row>
     <row r="118" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="4" t="s">
+      <c r="B118" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C118" s="5"/>
-      <c r="D118" s="4"/>
-      <c r="E118" s="6"/>
-      <c r="F118" s="5"/>
+      <c r="C118" s="6"/>
+      <c r="D118" s="5"/>
+      <c r="E118" s="10"/>
+      <c r="F118" s="6"/>
     </row>
     <row r="119" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="4" t="s">
+      <c r="B119" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C119" s="5"/>
-      <c r="D119" s="4"/>
-      <c r="E119" s="6"/>
-      <c r="F119" s="5"/>
+      <c r="C119" s="6"/>
+      <c r="D119" s="5"/>
+      <c r="E119" s="10"/>
+      <c r="F119" s="6"/>
     </row>
     <row r="120" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="4" t="s">
+      <c r="B120" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C120" s="5"/>
-      <c r="D120" s="4"/>
-      <c r="E120" s="6"/>
-      <c r="F120" s="5"/>
+      <c r="C120" s="6"/>
+      <c r="D120" s="5"/>
+      <c r="E120" s="10"/>
+      <c r="F120" s="6"/>
     </row>
     <row r="121" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="4" t="s">
+      <c r="B121" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C121" s="5"/>
-      <c r="D121" s="4"/>
-      <c r="E121" s="6"/>
-      <c r="F121" s="5"/>
+      <c r="C121" s="6"/>
+      <c r="D121" s="5"/>
+      <c r="E121" s="10"/>
+      <c r="F121" s="6"/>
     </row>
     <row r="122" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B122" s="4" t="s">
+      <c r="B122" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C122" s="5"/>
-      <c r="D122" s="4"/>
-      <c r="E122" s="6"/>
-      <c r="F122" s="5"/>
+      <c r="C122" s="6"/>
+      <c r="D122" s="5"/>
+      <c r="E122" s="10"/>
+      <c r="F122" s="6"/>
     </row>
     <row r="123" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B123" s="4" t="s">
+      <c r="B123" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C123" s="5"/>
-      <c r="D123" s="4" t="s">
+      <c r="C123" s="6"/>
+      <c r="D123" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E123" s="6"/>
-      <c r="F123" s="5"/>
+      <c r="E123" s="10"/>
+      <c r="F123" s="6"/>
     </row>
     <row r="124" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B124" s="4" t="s">
+      <c r="B124" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C124" s="5"/>
-      <c r="D124" s="4"/>
-      <c r="E124" s="6"/>
-      <c r="F124" s="5"/>
+      <c r="C124" s="6"/>
+      <c r="D124" s="5"/>
+      <c r="E124" s="10"/>
+      <c r="F124" s="6"/>
     </row>
     <row r="125" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B125" s="4" t="s">
+      <c r="B125" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C125" s="5"/>
-      <c r="D125" s="4"/>
-      <c r="E125" s="6"/>
-      <c r="F125" s="5"/>
+      <c r="C125" s="6"/>
+      <c r="D125" s="5"/>
+      <c r="E125" s="10"/>
+      <c r="F125" s="6"/>
     </row>
     <row r="126" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B126" s="4" t="s">
+      <c r="B126" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C126" s="5"/>
-      <c r="D126" s="4"/>
-      <c r="E126" s="6"/>
-      <c r="F126" s="5"/>
+      <c r="C126" s="6"/>
+      <c r="D126" s="5"/>
+      <c r="E126" s="10"/>
+      <c r="F126" s="6"/>
     </row>
     <row r="127" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B127" s="4" t="s">
+      <c r="B127" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C127" s="5"/>
-      <c r="D127" s="4"/>
-      <c r="E127" s="6"/>
-      <c r="F127" s="5"/>
+      <c r="C127" s="6"/>
+      <c r="D127" s="5"/>
+      <c r="E127" s="10"/>
+      <c r="F127" s="6"/>
     </row>
     <row r="128" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="4" t="s">
+      <c r="B128" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C128" s="5"/>
-      <c r="D128" s="4"/>
-      <c r="E128" s="6"/>
-      <c r="F128" s="5"/>
+      <c r="C128" s="6"/>
+      <c r="D128" s="5"/>
+      <c r="E128" s="10"/>
+      <c r="F128" s="6"/>
     </row>
     <row r="129" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B129" s="4" t="s">
+      <c r="B129" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C129" s="5"/>
-      <c r="D129" s="4"/>
-      <c r="E129" s="6"/>
-      <c r="F129" s="5"/>
+      <c r="C129" s="6"/>
+      <c r="D129" s="5"/>
+      <c r="E129" s="10"/>
+      <c r="F129" s="6"/>
     </row>
     <row r="130" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B130" s="4" t="s">
+      <c r="B130" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C130" s="5"/>
-      <c r="D130" s="4"/>
-      <c r="E130" s="6"/>
-      <c r="F130" s="5"/>
+      <c r="C130" s="6"/>
+      <c r="D130" s="5"/>
+      <c r="E130" s="10"/>
+      <c r="F130" s="6"/>
     </row>
     <row r="131" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B131" s="4" t="s">
+      <c r="B131" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C131" s="5"/>
-      <c r="D131" s="4"/>
-      <c r="E131" s="6"/>
-      <c r="F131" s="5"/>
+      <c r="C131" s="6"/>
+      <c r="D131" s="5"/>
+      <c r="E131" s="10"/>
+      <c r="F131" s="6"/>
     </row>
     <row r="132" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B132" s="4" t="s">
+      <c r="B132" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C132" s="5"/>
-      <c r="D132" s="4" t="s">
+      <c r="C132" s="6"/>
+      <c r="D132" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E132" s="6"/>
-      <c r="F132" s="5"/>
+      <c r="E132" s="10"/>
+      <c r="F132" s="6"/>
     </row>
     <row r="133" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B133" s="4" t="s">
+      <c r="B133" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C133" s="5"/>
-      <c r="D133" s="4"/>
-      <c r="E133" s="6"/>
-      <c r="F133" s="5"/>
+      <c r="C133" s="6"/>
+      <c r="D133" s="5"/>
+      <c r="E133" s="10"/>
+      <c r="F133" s="6"/>
     </row>
     <row r="134" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B134" s="4" t="s">
+      <c r="B134" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C134" s="5"/>
-      <c r="D134" s="4"/>
-      <c r="E134" s="6"/>
-      <c r="F134" s="5"/>
+      <c r="C134" s="6"/>
+      <c r="D134" s="5"/>
+      <c r="E134" s="10"/>
+      <c r="F134" s="6"/>
     </row>
     <row r="135" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B135" s="4" t="s">
+      <c r="B135" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C135" s="5"/>
-      <c r="D135" s="4"/>
-      <c r="E135" s="6"/>
-      <c r="F135" s="5"/>
+      <c r="C135" s="6"/>
+      <c r="D135" s="5"/>
+      <c r="E135" s="10"/>
+      <c r="F135" s="6"/>
     </row>
     <row r="136" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B136" s="4" t="s">
+      <c r="B136" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C136" s="5"/>
-      <c r="D136" s="4"/>
-      <c r="E136" s="6"/>
-      <c r="F136" s="5"/>
+      <c r="C136" s="6"/>
+      <c r="D136" s="5"/>
+      <c r="E136" s="10"/>
+      <c r="F136" s="6"/>
     </row>
     <row r="137" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B137" s="4" t="s">
+      <c r="B137" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C137" s="5"/>
-      <c r="D137" s="4"/>
-      <c r="E137" s="6"/>
-      <c r="F137" s="5"/>
+      <c r="C137" s="6"/>
+      <c r="D137" s="5"/>
+      <c r="E137" s="10"/>
+      <c r="F137" s="6"/>
     </row>
     <row r="138" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B138" s="4" t="s">
+      <c r="B138" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C138" s="5"/>
-      <c r="D138" s="4"/>
-      <c r="E138" s="6"/>
-      <c r="F138" s="5"/>
+      <c r="C138" s="6"/>
+      <c r="D138" s="5"/>
+      <c r="E138" s="10"/>
+      <c r="F138" s="6"/>
     </row>
     <row r="139" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B139" s="4" t="s">
+      <c r="B139" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C139" s="5"/>
-      <c r="D139" s="4"/>
-      <c r="E139" s="6"/>
-      <c r="F139" s="5"/>
+      <c r="C139" s="6"/>
+      <c r="D139" s="5"/>
+      <c r="E139" s="10"/>
+      <c r="F139" s="6"/>
     </row>
     <row r="140" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B140" s="4" t="s">
+      <c r="B140" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C140" s="5"/>
-      <c r="D140" s="4"/>
-      <c r="E140" s="6"/>
-      <c r="F140" s="5"/>
+      <c r="C140" s="6"/>
+      <c r="D140" s="5"/>
+      <c r="E140" s="10"/>
+      <c r="F140" s="6"/>
     </row>
     <row r="141" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B141" s="4" t="s">
+      <c r="B141" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C141" s="5"/>
-      <c r="D141" s="4" t="s">
+      <c r="C141" s="6"/>
+      <c r="D141" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E141" s="6"/>
-      <c r="F141" s="5"/>
+      <c r="E141" s="10"/>
+      <c r="F141" s="6"/>
     </row>
     <row r="142" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B142" s="4" t="s">
+      <c r="B142" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C142" s="5"/>
-      <c r="D142" s="4"/>
-      <c r="E142" s="6"/>
-      <c r="F142" s="5"/>
+      <c r="C142" s="6"/>
+      <c r="D142" s="5"/>
+      <c r="E142" s="10"/>
+      <c r="F142" s="6"/>
     </row>
     <row r="143" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B143" s="4" t="s">
+      <c r="B143" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C143" s="5"/>
-      <c r="D143" s="4"/>
-      <c r="E143" s="6"/>
-      <c r="F143" s="5"/>
+      <c r="C143" s="6"/>
+      <c r="D143" s="5"/>
+      <c r="E143" s="10"/>
+      <c r="F143" s="6"/>
     </row>
     <row r="144" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B144" s="4" t="s">
+      <c r="B144" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C144" s="5"/>
-      <c r="D144" s="4"/>
-      <c r="E144" s="6"/>
-      <c r="F144" s="5"/>
+      <c r="C144" s="6"/>
+      <c r="D144" s="5"/>
+      <c r="E144" s="10"/>
+      <c r="F144" s="6"/>
     </row>
     <row r="145" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B145" s="4" t="s">
+      <c r="B145" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C145" s="5"/>
-      <c r="D145" s="4"/>
-      <c r="E145" s="6"/>
-      <c r="F145" s="5"/>
+      <c r="C145" s="6"/>
+      <c r="D145" s="5"/>
+      <c r="E145" s="10"/>
+      <c r="F145" s="6"/>
     </row>
     <row r="146" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B146" s="4" t="s">
+      <c r="B146" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C146" s="5"/>
-      <c r="D146" s="4"/>
-      <c r="E146" s="6"/>
-      <c r="F146" s="5"/>
+      <c r="C146" s="6"/>
+      <c r="D146" s="5"/>
+      <c r="E146" s="10"/>
+      <c r="F146" s="6"/>
     </row>
     <row r="147" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B147" s="4" t="s">
+      <c r="B147" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C147" s="5"/>
-      <c r="D147" s="4"/>
-      <c r="E147" s="6"/>
-      <c r="F147" s="5"/>
+      <c r="C147" s="6"/>
+      <c r="D147" s="5"/>
+      <c r="E147" s="10"/>
+      <c r="F147" s="6"/>
     </row>
     <row r="148" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B148" s="4" t="s">
+      <c r="B148" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C148" s="5"/>
-      <c r="D148" s="4"/>
-      <c r="E148" s="6"/>
-      <c r="F148" s="5"/>
+      <c r="C148" s="6"/>
+      <c r="D148" s="5"/>
+      <c r="E148" s="10"/>
+      <c r="F148" s="6"/>
     </row>
     <row r="149" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B149" s="4" t="s">
+      <c r="B149" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C149" s="5"/>
-      <c r="D149" s="4"/>
-      <c r="E149" s="6"/>
-      <c r="F149" s="5"/>
+      <c r="C149" s="6"/>
+      <c r="D149" s="5"/>
+      <c r="E149" s="10"/>
+      <c r="F149" s="6"/>
     </row>
     <row r="150" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B150" s="4" t="s">
+      <c r="B150" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C150" s="5"/>
-      <c r="D150" s="4" t="s">
+      <c r="C150" s="6"/>
+      <c r="D150" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E150" s="6"/>
-      <c r="F150" s="5"/>
+      <c r="E150" s="10"/>
+      <c r="F150" s="6"/>
     </row>
     <row r="151" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B151" s="4" t="s">
+      <c r="B151" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C151" s="5"/>
-      <c r="D151" s="4"/>
-      <c r="E151" s="6"/>
-      <c r="F151" s="5"/>
+      <c r="C151" s="6"/>
+      <c r="D151" s="5"/>
+      <c r="E151" s="10"/>
+      <c r="F151" s="6"/>
     </row>
     <row r="152" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B152" s="4" t="s">
+      <c r="B152" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C152" s="5"/>
-      <c r="D152" s="4"/>
-      <c r="E152" s="6"/>
-      <c r="F152" s="5"/>
+      <c r="C152" s="6"/>
+      <c r="D152" s="5"/>
+      <c r="E152" s="10"/>
+      <c r="F152" s="6"/>
     </row>
     <row r="153" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B153" s="4" t="s">
+      <c r="B153" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C153" s="5"/>
-      <c r="D153" s="4"/>
-      <c r="E153" s="6"/>
-      <c r="F153" s="5"/>
+      <c r="C153" s="6"/>
+      <c r="D153" s="5"/>
+      <c r="E153" s="10"/>
+      <c r="F153" s="6"/>
     </row>
     <row r="154" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B154" s="4" t="s">
+      <c r="B154" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C154" s="5"/>
-      <c r="D154" s="4"/>
-      <c r="E154" s="6"/>
-      <c r="F154" s="5"/>
+      <c r="C154" s="6"/>
+      <c r="D154" s="5"/>
+      <c r="E154" s="10"/>
+      <c r="F154" s="6"/>
     </row>
     <row r="155" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B155" s="4" t="s">
+      <c r="B155" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C155" s="5"/>
-      <c r="D155" s="4"/>
-      <c r="E155" s="6"/>
-      <c r="F155" s="5"/>
+      <c r="C155" s="6"/>
+      <c r="D155" s="5"/>
+      <c r="E155" s="10"/>
+      <c r="F155" s="6"/>
     </row>
     <row r="156" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B156" s="4" t="s">
+      <c r="B156" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C156" s="5"/>
-      <c r="D156" s="4"/>
-      <c r="E156" s="6"/>
-      <c r="F156" s="5"/>
+      <c r="C156" s="6"/>
+      <c r="D156" s="5"/>
+      <c r="E156" s="10"/>
+      <c r="F156" s="6"/>
     </row>
     <row r="157" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B157" s="4" t="s">
+      <c r="B157" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C157" s="5"/>
-      <c r="D157" s="4" t="s">
+      <c r="C157" s="6"/>
+      <c r="D157" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="E157" s="6"/>
-      <c r="F157" s="5"/>
+      <c r="E157" s="10"/>
+      <c r="F157" s="6"/>
     </row>
     <row r="158" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B158" s="4" t="s">
+      <c r="B158" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C158" s="5"/>
-      <c r="D158" s="4"/>
-      <c r="E158" s="6"/>
-      <c r="F158" s="5"/>
+      <c r="C158" s="6"/>
+      <c r="D158" s="5"/>
+      <c r="E158" s="10"/>
+      <c r="F158" s="6"/>
     </row>
     <row r="159" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B159" s="4" t="s">
+      <c r="B159" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C159" s="5"/>
-      <c r="D159" s="4"/>
-      <c r="E159" s="6"/>
-      <c r="F159" s="5"/>
+      <c r="C159" s="6"/>
+      <c r="D159" s="5"/>
+      <c r="E159" s="10"/>
+      <c r="F159" s="6"/>
     </row>
     <row r="160" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B160" s="4" t="s">
+      <c r="B160" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C160" s="5"/>
-      <c r="D160" s="4"/>
-      <c r="E160" s="6"/>
-      <c r="F160" s="5"/>
+      <c r="C160" s="6"/>
+      <c r="D160" s="5"/>
+      <c r="E160" s="10"/>
+      <c r="F160" s="6"/>
     </row>
     <row r="161" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B161" s="4" t="s">
+      <c r="B161" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C161" s="5"/>
-      <c r="D161" s="4"/>
-      <c r="E161" s="6"/>
-      <c r="F161" s="5"/>
+      <c r="C161" s="6"/>
+      <c r="D161" s="5"/>
+      <c r="E161" s="10"/>
+      <c r="F161" s="6"/>
     </row>
     <row r="162" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B162" s="4" t="s">
+      <c r="B162" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C162" s="5"/>
-      <c r="D162" s="4" t="s">
+      <c r="C162" s="6"/>
+      <c r="D162" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="E162" s="6"/>
-      <c r="F162" s="5"/>
+      <c r="E162" s="10"/>
+      <c r="F162" s="6"/>
     </row>
     <row r="163" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B163" s="4" t="s">
+      <c r="B163" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C163" s="5"/>
-      <c r="D163" s="4"/>
-      <c r="E163" s="6"/>
-      <c r="F163" s="5"/>
+      <c r="C163" s="6"/>
+      <c r="D163" s="5"/>
+      <c r="E163" s="10"/>
+      <c r="F163" s="6"/>
     </row>
     <row r="164" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B164" s="4" t="s">
+      <c r="B164" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C164" s="5"/>
-      <c r="D164" s="4"/>
-      <c r="E164" s="6"/>
-      <c r="F164" s="5"/>
+      <c r="C164" s="6"/>
+      <c r="D164" s="5"/>
+      <c r="E164" s="10"/>
+      <c r="F164" s="6"/>
     </row>
     <row r="165" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B165" s="4" t="s">
+      <c r="B165" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C165" s="5"/>
-      <c r="D165" s="4"/>
-      <c r="E165" s="6"/>
-      <c r="F165" s="5"/>
+      <c r="C165" s="6"/>
+      <c r="D165" s="5"/>
+      <c r="E165" s="10"/>
+      <c r="F165" s="6"/>
     </row>
     <row r="166" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B166" s="4" t="s">
+      <c r="B166" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C166" s="5"/>
-      <c r="D166" s="4"/>
-      <c r="E166" s="6"/>
-      <c r="F166" s="5"/>
+      <c r="C166" s="6"/>
+      <c r="D166" s="5"/>
+      <c r="E166" s="10"/>
+      <c r="F166" s="6"/>
     </row>
     <row r="167" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B167" s="4" t="s">
+      <c r="B167" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C167" s="5"/>
-      <c r="D167" s="4"/>
-      <c r="E167" s="6"/>
-      <c r="F167" s="5"/>
+      <c r="C167" s="6"/>
+      <c r="D167" s="5"/>
+      <c r="E167" s="10"/>
+      <c r="F167" s="6"/>
     </row>
     <row r="168" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B168" s="4" t="s">
+      <c r="B168" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C168" s="5"/>
-      <c r="D168" s="4"/>
-      <c r="E168" s="6"/>
-      <c r="F168" s="5"/>
+      <c r="C168" s="6"/>
+      <c r="D168" s="5"/>
+      <c r="E168" s="10"/>
+      <c r="F168" s="6"/>
     </row>
     <row r="169" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B169" s="4" t="s">
+      <c r="B169" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C169" s="5"/>
-      <c r="D169" s="4"/>
-      <c r="E169" s="6"/>
-      <c r="F169" s="5"/>
+      <c r="C169" s="6"/>
+      <c r="D169" s="5"/>
+      <c r="E169" s="10"/>
+      <c r="F169" s="6"/>
     </row>
     <row r="170" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B170" s="4" t="s">
+      <c r="B170" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C170" s="5"/>
-      <c r="D170" s="4"/>
-      <c r="E170" s="6"/>
-      <c r="F170" s="5"/>
+      <c r="C170" s="6"/>
+      <c r="D170" s="5"/>
+      <c r="E170" s="10"/>
+      <c r="F170" s="6"/>
     </row>
     <row r="171" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B171" s="4" t="s">
+      <c r="B171" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C171" s="5"/>
-      <c r="D171" s="4" t="s">
+      <c r="C171" s="6"/>
+      <c r="D171" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E171" s="6"/>
-      <c r="F171" s="5"/>
+      <c r="E171" s="10"/>
+      <c r="F171" s="6"/>
     </row>
     <row r="172" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B172" s="4" t="s">
+      <c r="B172" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C172" s="5"/>
-      <c r="D172" s="4"/>
-      <c r="E172" s="6"/>
-      <c r="F172" s="5"/>
+      <c r="C172" s="6"/>
+      <c r="D172" s="5"/>
+      <c r="E172" s="10"/>
+      <c r="F172" s="6"/>
     </row>
     <row r="173" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B173" s="4" t="s">
+      <c r="B173" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C173" s="5"/>
-      <c r="D173" s="4"/>
-      <c r="E173" s="6"/>
-      <c r="F173" s="5"/>
+      <c r="C173" s="6"/>
+      <c r="D173" s="5"/>
+      <c r="E173" s="10"/>
+      <c r="F173" s="6"/>
     </row>
     <row r="174" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B174" s="4" t="s">
+      <c r="B174" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C174" s="5"/>
-      <c r="D174" s="4"/>
-      <c r="E174" s="6"/>
-      <c r="F174" s="5"/>
+      <c r="C174" s="6"/>
+      <c r="D174" s="5"/>
+      <c r="E174" s="10"/>
+      <c r="F174" s="6"/>
     </row>
     <row r="175" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B175" s="4" t="s">
+      <c r="B175" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C175" s="5"/>
-      <c r="D175" s="4"/>
-      <c r="E175" s="6"/>
-      <c r="F175" s="5"/>
+      <c r="C175" s="6"/>
+      <c r="D175" s="5"/>
+      <c r="E175" s="10"/>
+      <c r="F175" s="6"/>
     </row>
     <row r="176" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B176" s="4" t="s">
+      <c r="B176" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C176" s="5"/>
-      <c r="D176" s="4"/>
-      <c r="E176" s="6"/>
-      <c r="F176" s="5"/>
+      <c r="C176" s="6"/>
+      <c r="D176" s="5"/>
+      <c r="E176" s="10"/>
+      <c r="F176" s="6"/>
     </row>
     <row r="177" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B177" s="4" t="s">
+      <c r="B177" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C177" s="5"/>
-      <c r="D177" s="4"/>
-      <c r="E177" s="6"/>
-      <c r="F177" s="5"/>
+      <c r="C177" s="6"/>
+      <c r="D177" s="5"/>
+      <c r="E177" s="10"/>
+      <c r="F177" s="6"/>
     </row>
     <row r="178" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B178" s="4" t="s">
+      <c r="B178" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C178" s="5"/>
-      <c r="D178" s="4"/>
-      <c r="E178" s="6"/>
-      <c r="F178" s="5"/>
+      <c r="C178" s="6"/>
+      <c r="D178" s="5"/>
+      <c r="E178" s="10"/>
+      <c r="F178" s="6"/>
     </row>
     <row r="179" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B179" s="4" t="s">
+      <c r="B179" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C179" s="5"/>
-      <c r="D179" s="4"/>
-      <c r="E179" s="6"/>
-      <c r="F179" s="5"/>
+      <c r="C179" s="6"/>
+      <c r="D179" s="5"/>
+      <c r="E179" s="10"/>
+      <c r="F179" s="6"/>
     </row>
     <row r="180" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B180" s="4" t="s">
+      <c r="B180" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C180" s="5"/>
-      <c r="D180" s="4"/>
-      <c r="E180" s="6"/>
-      <c r="F180" s="5"/>
+      <c r="C180" s="6"/>
+      <c r="D180" s="5"/>
+      <c r="E180" s="10"/>
+      <c r="F180" s="6"/>
     </row>
     <row r="181" spans="2:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B181" s="4" t="s">
+      <c r="B181" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C181" s="5"/>
-      <c r="D181" s="4"/>
-      <c r="E181" s="6"/>
-      <c r="F181" s="5"/>
+      <c r="C181" s="6"/>
+      <c r="D181" s="5"/>
+      <c r="E181" s="10"/>
+      <c r="F181" s="6"/>
     </row>
     <row r="182" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>

</xml_diff>